<commit_message>
tinkered with simulated annealing
</commit_message>
<xml_diff>
--- a/cambridge-colleges-coords.xlsx
+++ b/cambridge-colleges-coords.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lathanliou/Desktop/Academic/DataProjects/cambridge-colleges/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF89ECF-7DE9-6F41-A8AD-D918D013444E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415CE446-6D61-BA4B-BA47-3AD992A6B446}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="1960" windowWidth="26840" windowHeight="14580" xr2:uid="{A98FDA03-0B5D-A14C-9313-971F622D1C76}"/>
+    <workbookView xWindow="1580" yWindow="1900" windowWidth="26840" windowHeight="14580" xr2:uid="{A98FDA03-0B5D-A14C-9313-971F622D1C76}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -610,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80B1294B-4F6D-A84E-AEB7-4840E47F9D8C}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -732,7 +732,7 @@
         <v>0.1135917</v>
       </c>
       <c r="E7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.25">

</xml_diff>